<commit_message>
Create base structure and Login tests
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70A3594-BCD5-4FD3-8A0D-489A53D8DB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3162A2-3D74-4F6C-BB36-34828ACFBFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Login with correct user</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
     <t>Accounts</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Use cucumber?</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -525,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B76C8-E645-4FAC-B88B-979A0DC02C71}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,19 +545,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -567,51 +567,57 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>11</v>
       </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
         <v>39</v>
@@ -619,29 +625,29 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -657,26 +663,26 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,31 +698,31 @@
         <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
+      <c r="A19" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
       <c r="B21" t="s">
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -724,7 +730,7 @@
         <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,7 +746,7 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -748,21 +754,24 @@
         <v>32</v>
       </c>
       <c r="E25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+      <c r="E26" t="s">
         <v>33</v>
       </c>
-      <c r="E26" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -770,26 +779,15 @@
         <v>41</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
       <c r="E28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Create and Read tests for Accounts module
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3162A2-3D74-4F6C-BB36-34828ACFBFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDCE5C2-F994-43DF-9D82-E436B15375DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -188,12 +188,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,9 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,7 +535,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -567,7 +574,7 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E4" t="s">
@@ -578,7 +585,7 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E5" t="s">
@@ -592,6 +599,9 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E6" t="s">
         <v>38</v>
       </c>
@@ -610,6 +620,9 @@
       </c>
       <c r="C8" t="s">
         <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Complete tests for Accounts module
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDCE5C2-F994-43DF-9D82-E436B15375DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EAE0E-C474-4084-A77B-2BBF294BA48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Delete new account</t>
   </si>
   <si>
-    <t>Edit existing</t>
-  </si>
-  <si>
     <t>Module</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Edit existing account</t>
+  </si>
+  <si>
+    <t>Check error messages on empty acc creation</t>
   </si>
 </sst>
 </file>
@@ -532,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B76C8-E645-4FAC-B88B-979A0DC02C71}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,19 +555,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -575,10 +578,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -586,10 +589,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -600,18 +603,21 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -619,21 +625,24 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -641,166 +650,177 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>7</v>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="E25" t="s">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create Page Steps for Contacts
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0EAE0E-C474-4084-A77B-2BBF294BA48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632887B6-8C1C-447C-80A2-F9234284C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Contacts</t>
   </si>
   <si>
-    <t>Cases</t>
-  </si>
-  <si>
     <t>API</t>
   </si>
   <si>
@@ -101,21 +98,9 @@
     <t>Delete existing contact</t>
   </si>
   <si>
-    <t>Create new case</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Read existing case</t>
-  </si>
-  <si>
-    <t>Edit existing case</t>
-  </si>
-  <si>
-    <t>Delete existing case</t>
-  </si>
-  <si>
     <t>Create lead with all main info</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
   </si>
   <si>
     <t>Create New Contact</t>
-  </si>
-  <si>
-    <t>Create New Case</t>
   </si>
   <si>
     <t>Type</t>
@@ -535,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B76C8-E645-4FAC-B88B-979A0DC02C71}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -555,19 +537,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -578,10 +560,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -589,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -600,68 +582,71 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -669,158 +654,115 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>28</v>
       </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
       <c r="E23" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>29</v>
       </c>
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
       <c r="E24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create BaseAPI Test for Create New Account
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D6D8AD-6B00-47CF-A1EB-7344FCE0C756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6EFE6-0B50-4A34-88E5-5D9CA53D3F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -59,9 +59,6 @@
     <t>API</t>
   </si>
   <si>
-    <t>Leads</t>
-  </si>
-  <si>
     <t>Create new account with all fields</t>
   </si>
   <si>
@@ -98,18 +95,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Read existing lead</t>
-  </si>
-  <si>
-    <t>Edit exsiting lead</t>
-  </si>
-  <si>
-    <t>Delete existing lead</t>
-  </si>
-  <si>
-    <t>Create lead with empty fields</t>
-  </si>
-  <si>
     <t>e2e</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>Check error messages on empty contact creation</t>
   </si>
   <si>
-    <t>Create lead</t>
-  </si>
-  <si>
     <t>Create Contact</t>
   </si>
   <si>
@@ -165,6 +147,27 @@
   </si>
   <si>
     <t>Delete Contact</t>
+  </si>
+  <si>
+    <t>Get Contacts List</t>
+  </si>
+  <si>
+    <t>Create Account</t>
+  </si>
+  <si>
+    <t>Read Account</t>
+  </si>
+  <si>
+    <t>Edit Account</t>
+  </si>
+  <si>
+    <t>Delete Account</t>
+  </si>
+  <si>
+    <t>Create account with empty fields</t>
+  </si>
+  <si>
+    <t>Get Accounts List</t>
   </si>
 </sst>
 </file>
@@ -532,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B76C8-E645-4FAC-B88B-979A0DC02C71}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,19 +555,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -575,10 +578,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -586,10 +589,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -597,71 +600,71 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -669,68 +672,68 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,79 +743,85 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
       <c r="B28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
@@ -820,13 +829,35 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>24</v>
+      <c r="E31" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete tests for Accounts API
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF6EFE6-0B50-4A34-88E5-5D9CA53D3F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F690F7E0-A586-4AF8-91FD-BE20FFB891A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B76C8-E645-4FAC-B88B-979A0DC02C71}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,6 +748,9 @@
       <c r="B19" t="s">
         <v>38</v>
       </c>
+      <c r="D19" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E19" t="s">
         <v>23</v>
       </c>
@@ -756,6 +759,9 @@
       <c r="B20" t="s">
         <v>39</v>
       </c>
+      <c r="D20" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E20" t="s">
         <v>23</v>
       </c>
@@ -764,6 +770,9 @@
       <c r="B21" t="s">
         <v>40</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E21" t="s">
         <v>24</v>
       </c>
@@ -772,6 +781,9 @@
       <c r="B22" t="s">
         <v>41</v>
       </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E22" t="s">
         <v>24</v>
       </c>
@@ -780,6 +792,9 @@
       <c r="B23" t="s">
         <v>42</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E23" t="s">
         <v>24</v>
       </c>
@@ -787,6 +802,9 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>43</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E24" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Add API Tests for Contacts
</commit_message>
<xml_diff>
--- a/testCases.xlsx
+++ b/testCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\FinalProject\salesforceAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F690F7E0-A586-4AF8-91FD-BE20FFB891A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E5936-3660-408D-B445-94B64B351BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{A22BBDC7-0268-45F5-9AA7-D17F09F61C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>Salesforce Test Checklist</t>
   </si>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -817,6 +817,9 @@
       <c r="B25" t="s">
         <v>33</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E25" t="s">
         <v>23</v>
       </c>
@@ -825,6 +828,9 @@
       <c r="B26" t="s">
         <v>34</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E26" t="s">
         <v>23</v>
       </c>
@@ -833,6 +839,9 @@
       <c r="B27" t="s">
         <v>35</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E27" t="s">
         <v>24</v>
       </c>
@@ -841,6 +850,9 @@
       <c r="B28" t="s">
         <v>36</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E28" t="s">
         <v>24</v>
       </c>
@@ -848,6 +860,9 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>37</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>

</xml_diff>